<commit_message>
chiarimenti casi ID [45, 73 e 74]
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111ENGINNERING/Engineering_Ingegneria_Informatica_S.p.A/AREAS_ADTWEB/20.15.00/accreditamento-checklist_AREAS_ADTWEB.xlsx
+++ b/GATEWAY/S1#111ENGINNERING/Engineering_Ingegneria_Informatica_S.p.A/AREAS_ADTWEB/20.15.00/accreditamento-checklist_AREAS_ADTWEB.xlsx
@@ -392,9 +392,6 @@
 Per questo caso di test è richiesta la  sola descrizione del comportamento a fronte di un timeout, da inserire nella colonna "J" nominata come "GESTIONE ERRORE".</t>
   </si>
   <si>
-    <t>Viene segnalato un errore di timeout e si chiede all'utente di provare più tardi.</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_LDO_CT5_KO</t>
   </si>
   <si>
@@ -600,9 +597,6 @@
     <t>2.16.840.1.113883.2.9.2.150.4.4.54f26fc703f6752be3bda44d513722e874b071231429a5b83dc67249122a7b9e.67b9ce2cf9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>Viene segnalato all'operatore un problema sulla codifica della diagnosi selezionata. L'operatore non è autonomo nella risoluzione bensì è necessario un intervento di configurazione.</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_LDO_CT16_KO</t>
   </si>
   <si>
@@ -618,9 +612,6 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.150.4.4.54f26fc703f6752be3bda44d513722e874b071231429a5b83dc67249122a7b9e.5d30cc0b4b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>Viene segnalato all'operatore un problema sulla via di somministrazione di un farmaco somministrato. L'operatore non è autonomo nella risoluzione bensì è necessario un intervento di configurazione.</t>
   </si>
   <si>
     <t>ID TEST CASE OK</t>
@@ -723,6 +714,15 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.150.4.4.0ab9776ebbd089cbcd7530973f52084b84311fd5c462e14770605e085d54feaf.9b1038849d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Viene segnalato all'operatore un problema sulla codifica della diagnosi selezionata. Il referto non viene prodotto e il messaggio a video invita l'utente a contattare l'amministratore di sistema</t>
+  </si>
+  <si>
+    <t>Viene segnalato all'operatore un problema sulla via di somministrazione di un farmaco somministrato.  Il referto non viene prodotto e il messaggio a video invita l'utente a contattare l'amministratore di sistema</t>
+  </si>
+  <si>
+    <t>Viene segnalato un errore di timeout, ma il flusso applicativo prosegue con la produzione del referto</t>
   </si>
 </sst>
 </file>
@@ -2643,10 +2643,10 @@
   <dimension ref="A1:O873"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
+      <selection pane="bottomRight" activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2860,13 +2860,13 @@
         <v>44993</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H10" s="18" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="I10" s="18" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="J10" s="19"/>
       <c r="K10" s="19" t="s">
@@ -2897,13 +2897,13 @@
         <v>44993</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="H11" s="37" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="I11" s="18" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J11" s="19"/>
       <c r="K11" s="19" t="s">
@@ -2934,13 +2934,13 @@
         <v>44993</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="I12" s="18" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="J12" s="19"/>
       <c r="K12" s="19" t="s">
@@ -2971,13 +2971,13 @@
         <v>44993</v>
       </c>
       <c r="G13" s="18" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="H13" s="18" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="I13" s="18" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J13" s="19"/>
       <c r="K13" s="19" t="s">
@@ -3091,7 +3091,7 @@
       <c r="H16" s="18"/>
       <c r="I16" s="18"/>
       <c r="J16" s="19" t="s">
-        <v>51</v>
+        <v>153</v>
       </c>
       <c r="K16" s="19" t="s">
         <v>32</v>
@@ -3114,25 +3114,25 @@
         <v>29</v>
       </c>
       <c r="D17" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="16" t="s">
         <v>52</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>53</v>
       </c>
       <c r="F17" s="17">
         <v>44958.683935185189</v>
       </c>
       <c r="G17" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="H17" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="H17" s="18" t="s">
+      <c r="I17" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="I17" s="18" t="s">
+      <c r="J17" s="19" t="s">
         <v>56</v>
-      </c>
-      <c r="J17" s="19" t="s">
-        <v>57</v>
       </c>
       <c r="K17" s="19" t="s">
         <v>32</v>
@@ -3155,25 +3155,25 @@
         <v>29</v>
       </c>
       <c r="D18" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="16" t="s">
         <v>58</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>59</v>
       </c>
       <c r="F18" s="17">
         <v>44958.690949074073</v>
       </c>
       <c r="G18" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="H18" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="H18" s="18" t="s">
+      <c r="I18" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="I18" s="18" t="s">
+      <c r="J18" s="19" t="s">
         <v>62</v>
-      </c>
-      <c r="J18" s="19" t="s">
-        <v>63</v>
       </c>
       <c r="K18" s="19" t="s">
         <v>32</v>
@@ -3196,25 +3196,25 @@
         <v>29</v>
       </c>
       <c r="D19" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" s="16" t="s">
         <v>64</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>65</v>
       </c>
       <c r="F19" s="17">
         <v>44958.697060185186</v>
       </c>
       <c r="G19" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="H19" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="H19" s="18" t="s">
+      <c r="I19" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="I19" s="18" t="s">
-        <v>68</v>
-      </c>
       <c r="J19" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K19" s="19" t="s">
         <v>32</v>
@@ -3237,25 +3237,25 @@
         <v>29</v>
       </c>
       <c r="D20" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" s="16" t="s">
         <v>69</v>
-      </c>
-      <c r="E20" s="16" t="s">
-        <v>70</v>
       </c>
       <c r="F20" s="17">
         <v>44958.704756944448</v>
       </c>
       <c r="G20" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="H20" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="H20" s="18" t="s">
+      <c r="I20" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="I20" s="18" t="s">
+      <c r="J20" s="19" t="s">
         <v>73</v>
-      </c>
-      <c r="J20" s="19" t="s">
-        <v>74</v>
       </c>
       <c r="K20" s="19" t="s">
         <v>32</v>
@@ -3278,25 +3278,25 @@
         <v>29</v>
       </c>
       <c r="D21" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="E21" s="16" t="s">
         <v>75</v>
-      </c>
-      <c r="E21" s="16" t="s">
-        <v>76</v>
       </c>
       <c r="F21" s="17">
         <v>44958.710370370369</v>
       </c>
       <c r="G21" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="H21" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="H21" s="18" t="s">
+      <c r="I21" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="I21" s="18" t="s">
-        <v>79</v>
-      </c>
       <c r="J21" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K21" s="19" t="s">
         <v>32</v>
@@ -3319,25 +3319,25 @@
         <v>29</v>
       </c>
       <c r="D22" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="E22" s="16" t="s">
         <v>80</v>
-      </c>
-      <c r="E22" s="16" t="s">
-        <v>81</v>
       </c>
       <c r="F22" s="17">
         <v>44958.71974537037</v>
       </c>
       <c r="G22" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="H22" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="H22" s="18" t="s">
+      <c r="I22" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="I22" s="18" t="s">
+      <c r="J22" s="19" t="s">
         <v>84</v>
-      </c>
-      <c r="J22" s="19" t="s">
-        <v>85</v>
       </c>
       <c r="K22" s="19" t="s">
         <v>32</v>
@@ -3360,25 +3360,25 @@
         <v>29</v>
       </c>
       <c r="D23" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="E23" s="16" t="s">
         <v>86</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>87</v>
       </c>
       <c r="F23" s="17">
         <v>44958.724502314813</v>
       </c>
       <c r="G23" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="H23" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="H23" s="18" t="s">
+      <c r="I23" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="I23" s="18" t="s">
-        <v>90</v>
-      </c>
       <c r="J23" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K23" s="19" t="s">
         <v>32</v>
@@ -3401,31 +3401,31 @@
         <v>29</v>
       </c>
       <c r="D24" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="E24" s="16" t="s">
         <v>91</v>
-      </c>
-      <c r="E24" s="16" t="s">
-        <v>92</v>
       </c>
       <c r="F24" s="17">
         <v>44958.73033564815</v>
       </c>
       <c r="G24" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="H24" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="H24" s="18" t="s">
+      <c r="I24" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="I24" s="18" t="s">
+      <c r="J24" s="19" t="s">
         <v>95</v>
-      </c>
-      <c r="J24" s="19" t="s">
-        <v>96</v>
       </c>
       <c r="K24" s="19" t="s">
         <v>32</v>
       </c>
       <c r="L24" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M24" s="19"/>
       <c r="N24" s="20" t="s">
@@ -3444,25 +3444,25 @@
         <v>29</v>
       </c>
       <c r="D25" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="E25" s="16" t="s">
         <v>98</v>
-      </c>
-      <c r="E25" s="16" t="s">
-        <v>99</v>
       </c>
       <c r="F25" s="17">
         <v>44958.735335648147</v>
       </c>
       <c r="G25" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="H25" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="H25" s="18" t="s">
+      <c r="I25" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="I25" s="18" t="s">
-        <v>102</v>
-      </c>
       <c r="J25" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K25" s="19" t="s">
         <v>32</v>
@@ -3485,25 +3485,25 @@
         <v>29</v>
       </c>
       <c r="D26" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="E26" s="16" t="s">
         <v>103</v>
-      </c>
-      <c r="E26" s="16" t="s">
-        <v>104</v>
       </c>
       <c r="F26" s="17">
         <v>44958.740347222221</v>
       </c>
       <c r="G26" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="H26" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="H26" s="18" t="s">
+      <c r="I26" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="I26" s="18" t="s">
-        <v>107</v>
-      </c>
       <c r="J26" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K26" s="19" t="s">
         <v>32</v>
@@ -3526,25 +3526,25 @@
         <v>29</v>
       </c>
       <c r="D27" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="E27" s="16" t="s">
         <v>108</v>
-      </c>
-      <c r="E27" s="16" t="s">
-        <v>109</v>
       </c>
       <c r="F27" s="17">
         <v>44958.746111111112</v>
       </c>
       <c r="G27" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="H27" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="H27" s="18" t="s">
+      <c r="I27" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="I27" s="18" t="s">
-        <v>112</v>
-      </c>
       <c r="J27" s="19" t="s">
-        <v>113</v>
+        <v>151</v>
       </c>
       <c r="K27" s="19" t="s">
         <v>32</v>
@@ -3567,25 +3567,25 @@
         <v>29</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F28" s="17">
         <v>44958.751944444448</v>
       </c>
       <c r="G28" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="H28" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="I28" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="H28" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="I28" s="18" t="s">
-        <v>118</v>
-      </c>
       <c r="J28" s="19" t="s">
-        <v>119</v>
+        <v>152</v>
       </c>
       <c r="K28" s="19" t="s">
         <v>32</v>
@@ -13780,24 +13780,24 @@
         <v>14</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1">
       <c r="A2" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2" s="28" t="s">
         <v>122</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>123</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>124</v>
-      </c>
-      <c r="D2" s="28" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.25" customHeight="1">
@@ -13805,69 +13805,69 @@
         <v>29</v>
       </c>
       <c r="B3" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="C3" s="31" t="s">
-        <v>126</v>
-      </c>
       <c r="D3" s="28" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1">
       <c r="A4" s="29" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.25" customHeight="1">
       <c r="A5" s="29" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.25" customHeight="1">
       <c r="A6" s="29" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.25" customHeight="1">
       <c r="A7" s="33" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D7" s="32" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.25" customHeight="1"/>
@@ -14890,7 +14890,7 @@
     </row>
     <row r="2" spans="1:2" ht="14.25" customHeight="1">
       <c r="A2" s="36" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B2" s="36" t="s">
         <v>32</v>
@@ -14898,10 +14898,10 @@
     </row>
     <row r="3" spans="1:2" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B3" s="36" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25" customHeight="1">

</xml_diff>